<commit_message>
kss vs time done
</commit_message>
<xml_diff>
--- a/ID_SORTED/kss_vs_time.xlsx
+++ b/ID_SORTED/kss_vs_time.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Umar\Desktop\fyp_drowsiness\ID_SORTED\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C2E172-D881-4433-9F11-746B6DA8E33F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A11691D-0F3C-48CC-86DA-1F642975EA6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Post" sheetId="1" r:id="rId1"/>
-    <sheet name="Pre" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,20 +22,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Morning</t>
-  </si>
-  <si>
-    <t>Afternoon</t>
-  </si>
-  <si>
-    <t>Night</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -354,8 +339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,200 +518,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BBBE919-78A9-4A35-AB79-6FB7A4322E77}">
-  <dimension ref="A1:C17"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>5</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
-      <c r="C11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12">
-        <v>4</v>
-      </c>
-      <c r="C12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>4</v>
-      </c>
-      <c r="B13">
-        <v>6</v>
-      </c>
-      <c r="C13">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>5</v>
-      </c>
-      <c r="B14">
-        <v>4</v>
-      </c>
-      <c r="C14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>3</v>
-      </c>
-      <c r="B15">
-        <v>4</v>
-      </c>
-      <c r="C15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>4</v>
-      </c>
-      <c r="B16">
-        <v>6</v>
-      </c>
-      <c r="C16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>3</v>
-      </c>
-      <c r="B17">
-        <v>5</v>
-      </c>
-      <c r="C17">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>